<commit_message>
Batch 4 annotations & fix total score excel formula on all annotations
</commit_message>
<xml_diff>
--- a/annotated_dataset/output_batch_1.xlsx
+++ b/annotated_dataset/output_batch_1.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathu\Desktop\Courses\4NL3\paraphrasing_detection\annotated_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933FB10E-1848-49D3-93EA-C9B938E85C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B277B1A5-2DB8-4492-893B-4BC784579F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1251,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1293,7 +1306,8 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>0</v>
+        <f>0.6*C2+0.4*D2</f>
+        <v>0.24999999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -1308,7 +1322,8 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>0</v>
+        <f t="shared" ref="E3:E66" si="0">0.6*C3+0.4*D3</f>
+        <v>0.29249999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -1323,7 +1338,8 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.52454545454545454</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -1338,7 +1354,8 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.48</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -1353,7 +1370,8 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.32824933687002655</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -1368,6 +1386,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1383,7 +1402,8 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -1398,7 +1418,8 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
@@ -1413,7 +1434,8 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
@@ -1428,7 +1450,8 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -1443,7 +1466,8 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.27482517482517482</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1458,7 +1482,8 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.36363636363636359</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
@@ -1473,7 +1498,8 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
@@ -1488,7 +1514,8 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
@@ -1503,7 +1530,8 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.27</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -1518,7 +1546,8 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.14615384615384616</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1533,7 +1562,8 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.32727272727272722</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -1548,7 +1578,8 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -1563,7 +1594,8 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.47142857142857142</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -1578,7 +1610,8 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.54</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
@@ -1593,7 +1626,8 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
@@ -1608,7 +1642,8 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.27</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -1623,7 +1658,8 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.34117647058823525</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
@@ -1638,7 +1674,8 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.46495806150978564</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
@@ -1653,7 +1690,8 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
@@ -1668,7 +1706,8 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.49999999999999994</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1683,7 +1722,8 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.18571428571428569</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -1698,7 +1738,8 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
@@ -1713,7 +1754,8 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1728,7 +1770,8 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
@@ -1743,7 +1786,8 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -1758,7 +1802,8 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.30952380952380948</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
@@ -1773,7 +1818,8 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
@@ -1788,7 +1834,8 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.22499999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
@@ -1803,6 +1850,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1818,7 +1866,8 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.47571428571428576</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1833,7 +1882,8 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.21666666666666665</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
@@ -1848,7 +1898,8 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1863,7 +1914,8 @@
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.28214285714285708</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1878,7 +1930,8 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.30779220779220778</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -1893,7 +1946,8 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.4693181818181818</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
@@ -1908,7 +1962,8 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.48</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
@@ -1923,7 +1978,8 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -1938,7 +1994,8 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.52705882352941169</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
@@ -1953,7 +2010,8 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
@@ -1968,7 +2026,8 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
@@ -1983,6 +2042,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1998,7 +2058,8 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.38760638297872335</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
@@ -2013,7 +2074,8 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
@@ -2028,7 +2090,8 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2043,7 +2106,8 @@
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.51428571428571435</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.4">
@@ -2058,7 +2122,8 @@
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.54</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2073,7 +2138,8 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.25846153846153846</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2088,7 +2154,8 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -2103,7 +2170,8 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.55036363636363628</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2118,7 +2186,8 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.43750000000000006</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.4">
@@ -2133,7 +2202,8 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.4">
@@ -2148,7 +2218,8 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2163,7 +2234,8 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2178,7 +2250,8 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16071428571428567</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2193,7 +2266,8 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.25636363636363629</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.4">
@@ -2208,7 +2282,8 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.16000000000000003</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.4">
@@ -2223,6 +2298,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2238,7 +2314,8 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.49867172675521815</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -2253,7 +2330,8 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.40312500000000001</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2268,7 +2346,8 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2">
-        <v>0</v>
+        <f t="shared" ref="E67:E130" si="1">0.6*C67+0.4*D67</f>
+        <v>0.17571428571428568</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2283,6 +2362,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2298,7 +2378,8 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.37999999999999995</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2313,7 +2394,8 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.49499999999999994</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
@@ -2328,7 +2410,8 @@
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.47658914728682172</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2343,7 +2426,8 @@
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2358,7 +2442,8 @@
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.43269230769230765</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.4">
@@ -2373,7 +2458,8 @@
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -2388,7 +2474,8 @@
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3296842105263158</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -2403,7 +2490,8 @@
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.25772727272727275</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.4">
@@ -2418,7 +2506,8 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.47142857142857142</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2433,7 +2522,8 @@
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.40090909090909094</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.4">
@@ -2448,7 +2538,8 @@
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.4">
@@ -2463,7 +2554,8 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.42</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.4">
@@ -2478,7 +2570,8 @@
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.16000000000000003</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2493,7 +2586,8 @@
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.38181818181818178</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.4">
@@ -2508,7 +2602,8 @@
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -2523,7 +2618,8 @@
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.42428571428571421</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2538,7 +2634,8 @@
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3214285714285714</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.4">
@@ -2553,7 +2650,8 @@
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.16000000000000003</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.4">
@@ -2568,7 +2666,8 @@
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.4">
@@ -2583,7 +2682,8 @@
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.35357142857142859</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.4">
@@ -2598,7 +2698,8 @@
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2613,7 +2714,8 @@
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3736363636363636</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2628,7 +2730,8 @@
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.48375000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.4">
@@ -2643,7 +2746,8 @@
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.43750000000000006</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.4">
@@ -2658,7 +2762,8 @@
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3214285714285714</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2673,7 +2778,8 @@
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.42843137254901958</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
@@ -2688,7 +2794,8 @@
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.52758620689655167</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2703,7 +2810,8 @@
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.52272727272727271</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2718,7 +2826,8 @@
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.54</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.4">
@@ -2733,7 +2842,8 @@
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2748,7 +2858,8 @@
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.45999999999999996</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.4">
@@ -2763,7 +2874,8 @@
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2778,7 +2890,8 @@
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.8750000000000002E-2</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -2793,7 +2906,8 @@
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2808,7 +2922,8 @@
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.46153846153846156</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.4">
@@ -2823,7 +2938,8 @@
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.36</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.4">
@@ -2838,6 +2954,7 @@
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2853,7 +2970,8 @@
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.53359683794466395</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.4">
@@ -2868,7 +2986,8 @@
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.49999999999999994</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2883,7 +3002,8 @@
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2898,7 +3018,8 @@
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.35244755244755244</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.4">
@@ -2913,7 +3034,8 @@
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2928,7 +3050,8 @@
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.42</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -2943,6 +3066,7 @@
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2958,7 +3082,8 @@
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.10285714285714284</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.4">
@@ -2973,7 +3098,8 @@
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.21666666666666665</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -2988,7 +3114,8 @@
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.50756302521008401</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -3003,7 +3130,8 @@
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.43428571428571427</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.4">
@@ -3018,7 +3146,8 @@
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.17499999999999993</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3033,7 +3162,8 @@
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.4">
@@ -3048,7 +3178,8 @@
       </c>
       <c r="D119" s="2"/>
       <c r="E119" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.4">
@@ -3063,7 +3194,8 @@
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.33</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3078,7 +3210,8 @@
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3093,7 +3226,8 @@
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.35604395604395606</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -3108,7 +3242,8 @@
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.38769230769230761</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.4">
@@ -3123,7 +3258,8 @@
       </c>
       <c r="D124" s="2"/>
       <c r="E124" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3138,7 +3274,8 @@
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.48484848484848481</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3153,7 +3290,8 @@
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.4">
@@ -3168,7 +3306,8 @@
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3183,7 +3322,8 @@
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.39318181818181813</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.4">
@@ -3198,7 +3338,8 @@
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.4017857142857143</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3213,7 +3354,8 @@
       </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.40714285714285714</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -3228,7 +3370,8 @@
       </c>
       <c r="D131" s="2"/>
       <c r="E131" s="2">
-        <v>0</v>
+        <f t="shared" ref="E131:E146" si="2">0.6*C131+0.4*D131</f>
+        <v>0.39166666666666666</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3243,7 +3386,8 @@
       </c>
       <c r="D132" s="2"/>
       <c r="E132" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.49090909090909091</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3258,7 +3402,8 @@
       </c>
       <c r="D133" s="2"/>
       <c r="E133" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.49583333333333329</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
@@ -3273,7 +3418,8 @@
       </c>
       <c r="D134" s="2"/>
       <c r="E134" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.49047619047619045</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3288,7 +3434,8 @@
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.40714285714285714</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="102" x14ac:dyDescent="0.4">
@@ -3303,7 +3450,8 @@
       </c>
       <c r="D136" s="2"/>
       <c r="E136" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.14935064935064934</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.4">
@@ -3318,6 +3466,7 @@
       </c>
       <c r="D137" s="2"/>
       <c r="E137" s="2">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3333,7 +3482,8 @@
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.45396825396825397</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.4">
@@ -3348,7 +3498,8 @@
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.24999999999999994</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.4">
@@ -3363,7 +3514,8 @@
       </c>
       <c r="D140" s="2"/>
       <c r="E140" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
@@ -3378,7 +3530,8 @@
       </c>
       <c r="D141" s="2"/>
       <c r="E141" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.40343249427917621</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.4">
@@ -3393,7 +3546,8 @@
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3408,7 +3562,8 @@
       </c>
       <c r="D143" s="2"/>
       <c r="E143" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.4425</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -3423,7 +3578,8 @@
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.4">
@@ -3438,7 +3594,8 @@
       </c>
       <c r="D145" s="2"/>
       <c r="E145" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.4">
@@ -3453,7 +3610,8 @@
       </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>